<commit_message>
Login error catch, time and percentage
</commit_message>
<xml_diff>
--- a/listExcel/list.xlsx
+++ b/listExcel/list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KrawczyD\Documents\programming\puppeteer_0.3\listExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KrawczyD\Desktop\Puppeter_1.0_no_modules - Copy (2)\script\listExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3692B07E-48D9-407B-8C78-B0B77EAB936C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CFE7EC-68F9-4277-A29B-367F31D5F612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,7 +408,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3">
-        <v>13822917</v>
+        <v>1111</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -433,7 +433,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3">
+        <v>222</v>
+      </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -443,7 +445,9 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3">
+        <v>333</v>
+      </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -453,7 +457,9 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3">
+        <v>444</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -463,7 +469,9 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="3">
+        <v>555</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -670,10 +678,7 @@
       <c r="A31" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="javascript:ReportHelper.runReport(%22ActivityReport%22,%22SITE=1100|SFC=13822917%22,false,true,%22TR700%22,true)" xr:uid="{3F3C9AEF-3A0D-4094-8EA8-564BBEB34100}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>